<commit_message>
feat(excel-sync): Implement bidirectional Excel sync PoC with color detection
- Add ExcelClient with header color detection (PUSH/PULL)
- Add SnapshotManager for incremental change detection
- Add data fetchers for DefiLlama, Llamanodes, Publicnodes
- Add BlockchainsWatcher to orchestrate the sync process
- Add end-to-end tests for the bidirectional flow
- Update Excel file with a new row for testing
- Add report documenting the implementation and performance
</commit_message>
<xml_diff>
--- a/data/ARBITRAGEXPLUS2025.xlsx
+++ b/data/ARBITRAGEXPLUS2025.xlsx
@@ -1,28 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="BLOCKCHAINS" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="DEXES" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="ASSETS" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="POOLS" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="ROUTES" sheetId="5" state="visible" r:id="rId5"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="EXECUTIONS" sheetId="6" state="visible" r:id="rId6"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="CONFIG" sheetId="7" state="visible" r:id="rId7"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="ALERTS" sheetId="8" state="visible" r:id="rId8"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="ORACLES" sheetId="9" state="visible" r:id="rId9"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="STRATEGIES" sheetId="10" state="visible" r:id="rId10"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="FLASH_LOANS" sheetId="11" state="visible" r:id="rId11"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="METRICS" sheetId="12" state="visible" r:id="rId12"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="LOGS" sheetId="13" state="visible" r:id="rId13"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="ORACLE_ASSETS" sheetId="14" state="visible" r:id="rId14"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="ERROR_HANDLING_CONFIG" sheetId="15" state="visible" r:id="rId15"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="COLLECTORS_CONFIG" sheetId="16" state="visible" r:id="rId16"/>
+    <sheet name="BLOCKCHAINS" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="DEXES" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="ASSETS" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="POOLS" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="ROUTES" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet name="EXECUTIONS" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet name="CONFIG" sheetId="7" state="visible" r:id="rId7"/>
+    <sheet name="ALERTS" sheetId="8" state="visible" r:id="rId8"/>
+    <sheet name="ORACLES" sheetId="9" state="visible" r:id="rId9"/>
+    <sheet name="STRATEGIES" sheetId="10" state="visible" r:id="rId10"/>
+    <sheet name="FLASH_LOANS" sheetId="11" state="visible" r:id="rId11"/>
+    <sheet name="METRICS" sheetId="12" state="visible" r:id="rId12"/>
+    <sheet name="LOGS" sheetId="13" state="visible" r:id="rId13"/>
+    <sheet name="ORACLE_ASSETS" sheetId="14" state="visible" r:id="rId14"/>
+    <sheet name="ERROR_HANDLING_CONFIG" sheetId="15" state="visible" r:id="rId15"/>
+    <sheet name="COLLECTORS_CONFIG" sheetId="16" state="visible" r:id="rId16"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -468,7 +468,7 @@
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
   <cols>
     <col width="20" customWidth="1" min="1" max="1"/>
     <col width="20" customWidth="1" min="2" max="2"/>
@@ -981,7 +981,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>avalanche_43114</t>
+          <t>avalanche_test_1760873174</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -1004,7 +1004,7 @@
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>https://avalanche.llamarpc.com</t>
+          <t>https://avalanche.public-rpc.com</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
@@ -1012,19 +1012,131 @@
           <t>https://api.avax.network/ext/bc/C/rpc</t>
         </is>
       </c>
-      <c r="H5" t="inlineStr"/>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>https://rpc.ankr.com/avalanche</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>wss://avalanche.public-rpc.com</t>
+        </is>
+      </c>
       <c r="J5" t="inlineStr">
         <is>
           <t>https://snowtrace.io</t>
+        </is>
+      </c>
+      <c r="K5" t="n">
+        <v>2000</v>
+      </c>
+      <c r="L5" t="n">
+        <v>25</v>
+      </c>
+      <c r="M5" t="n">
+        <v>200</v>
+      </c>
+      <c r="N5" t="n">
+        <v>25</v>
+      </c>
+      <c r="O5" t="b">
+        <v>1</v>
+      </c>
+      <c r="P5" t="n">
+        <v>25</v>
+      </c>
+      <c r="Q5" t="n">
+        <v>2</v>
+      </c>
+      <c r="R5" t="n">
+        <v>15000000</v>
+      </c>
+      <c r="S5" t="inlineStr">
+        <is>
+          <t>0xcA11bde05977b3631167028862bE2a173976CA11</t>
+        </is>
+      </c>
+      <c r="T5" t="inlineStr">
+        <is>
+          <t>0x49D5c2BdFfac6CE2BFdB6640F4F80f226bc10bAB</t>
+        </is>
+      </c>
+      <c r="U5" t="inlineStr">
+        <is>
+          <t>0xB97EF9Ef8734C71904D8002F8b6Bc66Dd9c48a6E</t>
+        </is>
+      </c>
+      <c r="V5" t="inlineStr">
+        <is>
+          <t>0x9702230A8Ea53601f5cD2dc00fDBc13d4dF4A8c7</t>
+        </is>
+      </c>
+      <c r="W5" t="inlineStr">
+        <is>
+          <t>0xd586E7F844cEa2F87f50152665BCbc2C279D8d70</t>
+        </is>
+      </c>
+      <c r="X5" t="inlineStr">
+        <is>
+          <t>TraderJoe, Pangolin, SushiSwap, Curve</t>
+        </is>
+      </c>
+      <c r="Y5" t="inlineStr">
+        <is>
+          <t>Aave, Benqi, TraderJoe</t>
         </is>
       </c>
       <c r="Z5" t="n">
         <v>2927787936.222067</v>
       </c>
+      <c r="AC5" t="n">
+        <v>21000</v>
+      </c>
+      <c r="AD5" t="n">
+        <v>1</v>
+      </c>
+      <c r="AE5" t="b">
+        <v>1</v>
+      </c>
+      <c r="AF5" t="b">
+        <v>0</v>
+      </c>
+      <c r="AG5" t="b">
+        <v>0</v>
+      </c>
+      <c r="AH5" t="b">
+        <v>0</v>
+      </c>
       <c r="AI5" t="inlineStr">
         <is>
-          <t>HEALTHY</t>
-        </is>
+          <t>degraded</t>
+        </is>
+      </c>
+      <c r="AL5" t="inlineStr">
+        <is>
+          <t>synced</t>
+        </is>
+      </c>
+      <c r="AN5" t="n">
+        <v>99.5</v>
+      </c>
+      <c r="AO5" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="AP5" t="n">
+        <v>0</v>
+      </c>
+      <c r="AQ5" t="n">
+        <v>15000</v>
+      </c>
+      <c r="AR5" t="n">
+        <v>3</v>
+      </c>
+      <c r="AS5" t="n">
+        <v>10</v>
+      </c>
+      <c r="AT5" t="n">
+        <v>100</v>
       </c>
       <c r="AX5" t="b">
         <v>1</v>
@@ -1047,7 +1159,7 @@
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
   <cols>
     <col width="13" customWidth="1" min="1" max="1"/>
     <col width="15" customWidth="1" min="2" max="2"/>
@@ -1634,7 +1746,7 @@
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
   <cols>
     <col width="13" customWidth="1" min="1" max="1"/>
     <col width="15" customWidth="1" min="2" max="2"/>
@@ -2107,7 +2219,7 @@
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
   <cols>
     <col width="11" customWidth="1" min="1" max="1"/>
     <col width="13" customWidth="1" min="2" max="2"/>
@@ -2598,7 +2710,7 @@
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
   <cols>
     <col width="8" customWidth="1" min="1" max="1"/>
     <col width="11" customWidth="1" min="2" max="2"/>
@@ -2921,7 +3033,7 @@
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
   <cols>
     <col width="8" customWidth="1" min="1" max="1"/>
     <col width="12" customWidth="1" min="2" max="2"/>
@@ -6447,7 +6559,7 @@
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
   <cols>
     <col width="22" customWidth="1" min="1" max="1"/>
     <col width="12" customWidth="1" min="2" max="2"/>
@@ -6898,7 +7010,7 @@
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
   <cols>
     <col width="21" customWidth="1" min="1" max="1"/>
     <col width="9" customWidth="1" min="2" max="2"/>
@@ -7149,7 +7261,7 @@
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
   <cols>
     <col width="8" customWidth="1" min="1" max="1"/>
     <col width="6" customWidth="1" min="2" max="2"/>
@@ -8378,7 +8490,7 @@
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
   <cols>
     <col width="10" customWidth="1" min="1" max="1"/>
     <col width="8" customWidth="1" min="2" max="2"/>
@@ -10801,7 +10913,7 @@
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
   <cols>
     <col width="9" customWidth="1" min="1" max="1"/>
     <col width="8" customWidth="1" min="2" max="2"/>
@@ -11424,7 +11536,7 @@
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
   <cols>
     <col width="10" customWidth="1" min="1" max="1"/>
     <col width="8" customWidth="1" min="2" max="2"/>
@@ -12653,7 +12765,7 @@
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
   <cols>
     <col width="14" customWidth="1" min="1" max="1"/>
     <col width="10" customWidth="1" min="2" max="2"/>
@@ -12982,7 +13094,7 @@
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
   <cols>
     <col width="12" customWidth="1" min="1" max="1"/>
     <col width="7" customWidth="1" min="2" max="2"/>
@@ -13047,7 +13159,7 @@
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
   <cols>
     <col width="10" customWidth="1" min="1" max="1"/>
     <col width="6" customWidth="1" min="2" max="2"/>
@@ -13124,7 +13236,7 @@
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
   <cols>
     <col width="11" customWidth="1" min="1" max="1"/>
     <col width="13" customWidth="1" min="2" max="2"/>

</xml_diff>